<commit_message>
Added vertical connectors as an option
Vertical connectors, increased mech size by 1mm
</commit_message>
<xml_diff>
--- a/Projects/OMD_CAN_F4_UWB R3/BOM/Bill of Materials-OMD_CAN_F4_UWB.xlsx
+++ b/Projects/OMD_CAN_F4_UWB R3/BOM/Bill of Materials-OMD_CAN_F4_UWB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43170" windowHeight="22365" xr2:uid="{36F4CEEC-9069-4C4D-9835-2436CB68BA56}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43170" windowHeight="22365" xr2:uid="{7F3B8327-4F9E-46CE-8991-77375067DBC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-OMD_CAN_F4_UW" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="135">
   <si>
     <t>Comment</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>445-7438-1-ND, 445-7438-6-ND</t>
+  </si>
+  <si>
+    <t>JST_GH_V4</t>
+  </si>
+  <si>
+    <t>BM04B-GHS-TBT</t>
+  </si>
+  <si>
+    <t>CANV_CAN1, CANV_CAN2</t>
+  </si>
+  <si>
+    <t>455-1580-2-ND</t>
   </si>
   <si>
     <t>JST_GH_H4</t>
@@ -805,8 +817,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599CC4BA-5B4B-4225-9634-03164DF3B899}">
-  <dimension ref="A1:P25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE268F21-BABF-4685-A21D-50BA9CFAA4B3}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1296,10 +1308,10 @@
         <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>21</v>
@@ -1308,7 +1320,7 @@
         <v>21</v>
       </c>
       <c r="H12" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>22</v>
@@ -1318,31 +1330,31 @@
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="2" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="F13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1350,7 +1362,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>22</v>
@@ -1360,30 +1372,30 @@
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="2" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>21</v>
@@ -1402,7 +1414,7 @@
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1413,20 +1425,20 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F15" s="4" t="s">
         <v>21</v>
       </c>
@@ -1434,7 +1446,7 @@
         <v>21</v>
       </c>
       <c r="H15" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>22</v>
@@ -1444,30 +1456,30 @@
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="2" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>21</v>
@@ -1476,7 +1488,7 @@
         <v>21</v>
       </c>
       <c r="H16" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>22</v>
@@ -1486,30 +1498,30 @@
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="2" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>21</v>
@@ -1518,7 +1530,7 @@
         <v>21</v>
       </c>
       <c r="H17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>22</v>
@@ -1528,7 +1540,7 @@
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -1539,19 +1551,19 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>21</v>
@@ -1570,31 +1582,31 @@
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="2" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="F19" s="4" t="s">
         <v>21</v>
       </c>
@@ -1602,7 +1614,7 @@
         <v>21</v>
       </c>
       <c r="H19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>22</v>
@@ -1612,30 +1624,30 @@
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="2" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>21</v>
@@ -1647,14 +1659,14 @@
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -1665,31 +1677,31 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="3">
-        <v>2</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>21</v>
@@ -1710,13 +1722,13 @@
         <v>113</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>113</v>
@@ -1728,7 +1740,7 @@
         <v>21</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>22</v>
@@ -1738,7 +1750,7 @@
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1749,19 +1761,19 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>21</v>
@@ -1780,7 +1792,7 @@
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="4" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -1794,16 +1806,16 @@
         <v>122</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>21</v>
@@ -1822,7 +1834,7 @@
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="4" t="s">
-        <v>124</v>
+        <v>21</v>
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -1833,19 +1845,19 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>127</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>21</v>
@@ -1864,7 +1876,7 @@
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -1873,80 +1885,125 @@
         <v>21</v>
       </c>
     </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" tooltip="Component" display="'" xr:uid="{1212BEDB-8B4C-4589-99A0-539FD5ADF89D}"/>
-    <hyperlink ref="G2" tooltip="Manufacturer" display="'" xr:uid="{400AEA6E-4FBD-46DA-8141-60C8E22578CC}"/>
-    <hyperlink ref="L2" tooltip="Supplier" display="'490-13331-1-ND" xr:uid="{CC5D8C5F-1774-4C9F-B78F-7F1322AD14F2}"/>
-    <hyperlink ref="F3" tooltip="Component" display="'" xr:uid="{1FDEAFF4-AC38-4B40-BFE6-A3FFD1D9C557}"/>
-    <hyperlink ref="G3" tooltip="Manufacturer" display="'" xr:uid="{5F729FB9-D547-4ABD-8162-6025A02DBE4C}"/>
-    <hyperlink ref="L3" tooltip="Supplier" display="'490-10404-2-ND" xr:uid="{373D8211-AF88-493D-B1DE-9C79C0B7A98A}"/>
-    <hyperlink ref="F4" tooltip="Component" display="'" xr:uid="{D0BF1386-1416-4CD3-8B63-EA670B525F55}"/>
-    <hyperlink ref="G4" tooltip="Manufacturer" display="'" xr:uid="{C81C7CC1-A6F1-4334-8B59-1CB4B721F528}"/>
-    <hyperlink ref="L4" tooltip="Supplier" display="'490-10510-1-ND" xr:uid="{4BE0F8EC-047B-4C46-9CC7-A2E680D7DECE}"/>
-    <hyperlink ref="F5" tooltip="Component" display="'" xr:uid="{32A5388C-75B7-4E04-B2B2-0281195D9C6D}"/>
-    <hyperlink ref="G5" tooltip="Manufacturer" display="'" xr:uid="{698EEE0F-A6FC-408E-A976-D284CB21A3FC}"/>
-    <hyperlink ref="L5" tooltip="Supplier" display="'490-7229-2-ND" xr:uid="{D8EFD5F3-922E-4166-8DAB-6AC8830142DF}"/>
-    <hyperlink ref="F6" tooltip="Component" display="'" xr:uid="{CF72B24F-1A58-466C-A461-FECB47C60513}"/>
-    <hyperlink ref="G6" tooltip="Manufacturer" display="'" xr:uid="{044736E7-5B95-43ED-B4EC-3B66AF1CD320}"/>
-    <hyperlink ref="L6" tooltip="Supplier" display="'587-3766-1-ND" xr:uid="{F0FB1E3E-CDED-4C8D-8A75-65BC6C5D8E75}"/>
-    <hyperlink ref="F7" tooltip="Component" display="'" xr:uid="{3E957F4A-9B74-43EA-837F-0FDE00EF93BE}"/>
-    <hyperlink ref="G7" tooltip="Manufacturer" display="'" xr:uid="{AACEBDE8-8A3B-4E50-8A75-57F5D2CC088D}"/>
-    <hyperlink ref="L7" tooltip="Supplier" display="'311-1047-2-ND" xr:uid="{81872FD7-E685-4250-9951-88E2DB63EC66}"/>
-    <hyperlink ref="F8" tooltip="Component" display="'" xr:uid="{D08AE5D4-CBE5-4F13-9489-1F65F7E7B6A9}"/>
-    <hyperlink ref="G8" tooltip="Manufacturer" display="'" xr:uid="{CE0AE269-5767-4768-9028-3D134ECE98B4}"/>
-    <hyperlink ref="L8" tooltip="Supplier" display="'445-6007-2-ND" xr:uid="{DD6431D2-15D3-4BC5-9B41-1680CE74968D}"/>
-    <hyperlink ref="F9" tooltip="Component" display="'" xr:uid="{66AA083D-0193-45DF-A122-C27C75B2858F}"/>
-    <hyperlink ref="G9" tooltip="Manufacturer" display="'" xr:uid="{84C22513-5B71-48FB-BB65-3B59B8F394F7}"/>
-    <hyperlink ref="L9" tooltip="Supplier" display="'587-3766-1-ND" xr:uid="{FACBA814-79B2-4122-A8F2-82741401D7C6}"/>
-    <hyperlink ref="F10" tooltip="Component" display="'" xr:uid="{75421D07-DDA3-4C26-B834-F76558D79527}"/>
-    <hyperlink ref="G10" tooltip="Manufacturer" display="'" xr:uid="{E77755F2-ADDB-4B9F-A991-95B665457305}"/>
-    <hyperlink ref="L10" tooltip="Supplier" display="'445-7438-1-ND, 445-7438-6-ND" xr:uid="{CBAC2920-DECB-4250-8334-A6EA2907926B}"/>
-    <hyperlink ref="F11" tooltip="Component" display="'" xr:uid="{737D144E-BC57-4511-A388-9699B306BA5B}"/>
-    <hyperlink ref="G11" tooltip="Manufacturer" display="'" xr:uid="{638FA9AD-3743-4072-AB3F-7806D5B1068A}"/>
-    <hyperlink ref="L11" tooltip="Supplier" display="'455-1566-2-ND" xr:uid="{893C8324-F1F6-476E-B991-13B50CB520B1}"/>
-    <hyperlink ref="F12" tooltip="Component" display="'" xr:uid="{D8FAB8BB-34BA-4414-B6E4-B814065CBF01}"/>
-    <hyperlink ref="G12" tooltip="Manufacturer" display="'" xr:uid="{5C042B3E-7A07-4008-9FB0-F46E00A41391}"/>
-    <hyperlink ref="L12" tooltip="Supplier" display="'754-1802-1-ND" xr:uid="{7D642269-D395-4CD1-ABE2-4F43BA1D8C5B}"/>
-    <hyperlink ref="F13" tooltip="Component" display="'" xr:uid="{D0BFFF35-46DF-44FF-BD19-45416493E449}"/>
-    <hyperlink ref="G13" tooltip="Manufacturer" display="'" xr:uid="{F027B7EF-7B80-4328-A38F-0D6036FC74E3}"/>
-    <hyperlink ref="L13" tooltip="Supplier" display="'SM06B-SURS-TF(LF)(SN)-ND" xr:uid="{63595017-E2EA-4D88-A155-EBD04E590596}"/>
-    <hyperlink ref="F14" tooltip="Component" display="'" xr:uid="{FEC20B84-F621-40B9-A5EB-E8F3A46AFE63}"/>
-    <hyperlink ref="G14" tooltip="Manufacturer" display="'" xr:uid="{5967313A-648C-43A8-9B2C-4E584A2702DB}"/>
-    <hyperlink ref="L14" tooltip="Supplier" display="'P15980TR-ND" xr:uid="{85ADC265-9AF0-40DD-84C0-ECFF58495639}"/>
-    <hyperlink ref="F15" tooltip="Component" display="'" xr:uid="{088CD588-4010-4E64-BBD5-B85C1C201D99}"/>
-    <hyperlink ref="G15" tooltip="Manufacturer" display="'" xr:uid="{A83AB6A9-EF6B-4793-B56B-774CA1470DBE}"/>
-    <hyperlink ref="L15" tooltip="Supplier" display="'311-220LRCT-ND" xr:uid="{33559EEF-2E55-4CC5-91B0-CA76E00DC6B0}"/>
-    <hyperlink ref="F16" tooltip="Component" display="'" xr:uid="{41F228A1-3E66-40AD-A902-CB479E280A55}"/>
-    <hyperlink ref="G16" tooltip="Manufacturer" display="'" xr:uid="{E0F4331C-66AA-45DA-BED1-765500F16357}"/>
-    <hyperlink ref="L16" tooltip="Supplier" display="'311-1.00KLRCT-ND" xr:uid="{151A89E1-429E-41A6-85F3-E5F73308338B}"/>
-    <hyperlink ref="F17" tooltip="Component" display="'" xr:uid="{D23EC846-4464-4A0E-BC2A-56BF3A7A09C8}"/>
-    <hyperlink ref="G17" tooltip="Manufacturer" display="'" xr:uid="{E3CD8928-3414-4C9F-940D-D6D7B27D88D9}"/>
-    <hyperlink ref="L17" tooltip="Supplier" display="'311-10.0KLRCT-ND" xr:uid="{317C02F2-1768-4885-BCF6-4A99C975139A}"/>
-    <hyperlink ref="F18" tooltip="Component" display="'" xr:uid="{F2188398-2EF0-4CF8-B472-F4D066F8BAFB}"/>
-    <hyperlink ref="G18" tooltip="Manufacturer" display="'" xr:uid="{EFCDED98-D7CC-4C56-935C-596DEBDE008D}"/>
-    <hyperlink ref="L18" tooltip="Supplier" display="'311-120JRTR-ND" xr:uid="{A88288A4-7537-4BFB-AAA4-1A094CBF71B7}"/>
-    <hyperlink ref="F19" tooltip="Component" display="'" xr:uid="{C6F5090D-7D79-4787-8A31-D826DFCEF2B2}"/>
-    <hyperlink ref="G19" tooltip="Manufacturer" display="'" xr:uid="{AEE34832-3C85-4CFE-8CC8-901811314763}"/>
-    <hyperlink ref="L19" tooltip="Supplier" display="'576-3680-1-ND" xr:uid="{ED29BE47-BDBB-4D92-B90A-55051B07A538}"/>
-    <hyperlink ref="F20" tooltip="Component" display="'" xr:uid="{2655D11E-CF18-49BE-A147-8C6EE915B84B}"/>
-    <hyperlink ref="G20" tooltip="Manufacturer" display="'" xr:uid="{F9CE48E6-7172-480A-BAC0-14D6330D2E4A}"/>
-    <hyperlink ref="L20" tooltip="Supplier" display="'2393651" xr:uid="{F31916C8-F629-4538-B9E9-BDC735709D23}"/>
-    <hyperlink ref="F21" tooltip="Component" display="'" xr:uid="{1A42ECA4-81F4-4390-8122-71795EB15E24}"/>
-    <hyperlink ref="G21" tooltip="Manufacturer" display="'" xr:uid="{657B3A7C-BB41-4027-B287-F3EEB797A8EB}"/>
-    <hyperlink ref="L21" tooltip="Supplier" display="'568-8686-2-ND" xr:uid="{07C6EDD6-3054-41E5-91C4-564E24009384}"/>
-    <hyperlink ref="F22" tooltip="Component" display="'" xr:uid="{2F5C432A-1A8F-4E5B-89EB-A5AC5293478B}"/>
-    <hyperlink ref="G22" tooltip="Manufacturer" display="'" xr:uid="{7AEF85EB-00AE-4A8D-9714-9C31E2A33D61}"/>
-    <hyperlink ref="L22" tooltip="Supplier" display="'NUF2042XV6T1GOSDKR-ND" xr:uid="{46914172-05A6-4C5E-A988-A4E98BAEED4B}"/>
-    <hyperlink ref="F23" tooltip="Component" display="'" xr:uid="{29A8F6F1-21A6-4118-95D3-38D419537B39}"/>
-    <hyperlink ref="G23" tooltip="Manufacturer" display="'" xr:uid="{879390AE-792B-4588-A0AF-170D72B81212}"/>
-    <hyperlink ref="L23" tooltip="Supplier" display="'" xr:uid="{217F1D64-AC8F-496E-928E-9485879C1B9F}"/>
-    <hyperlink ref="F24" tooltip="Component" display="'" xr:uid="{31061370-E713-40CB-A221-021B3DE91D2B}"/>
-    <hyperlink ref="G24" tooltip="Manufacturer" display="'" xr:uid="{08A90E6A-FCB3-4EE3-9883-DA0E6F36749C}"/>
-    <hyperlink ref="L24" tooltip="Supplier" display="'1479-1002-2-ND" xr:uid="{8174EB08-CDFD-4741-8743-7889734F3984}"/>
-    <hyperlink ref="F25" tooltip="Component" display="'" xr:uid="{C9F487FB-89DC-428F-AB46-C4BD703E5A6F}"/>
-    <hyperlink ref="G25" tooltip="Manufacturer" display="'" xr:uid="{C287049F-44F2-4B95-95FB-5B7346AFCAC4}"/>
-    <hyperlink ref="L25" tooltip="Supplier" display="'887-1846-2-ND" xr:uid="{7B2380F8-6B1C-4194-9EC9-A84532AABD65}"/>
+    <hyperlink ref="F2" tooltip="Component" display="'" xr:uid="{68A442AD-18A8-4DBD-B0AA-DF6A9E7DC634}"/>
+    <hyperlink ref="G2" tooltip="Manufacturer" display="'" xr:uid="{21F63E0C-D1EC-4643-BDDA-58882E1D43C0}"/>
+    <hyperlink ref="L2" tooltip="Supplier" display="'490-13331-1-ND" xr:uid="{C5A8A894-33C6-4473-89FA-B9999A5C1E56}"/>
+    <hyperlink ref="F3" tooltip="Component" display="'" xr:uid="{AE138349-480C-4886-9DC6-B2A3079C5908}"/>
+    <hyperlink ref="G3" tooltip="Manufacturer" display="'" xr:uid="{082C5011-1428-4775-BC27-DE7D53006B29}"/>
+    <hyperlink ref="L3" tooltip="Supplier" display="'490-10404-2-ND" xr:uid="{5BF68FD7-61EA-43FC-BC9A-E0070022258A}"/>
+    <hyperlink ref="F4" tooltip="Component" display="'" xr:uid="{AAF4FC7A-0D81-4CF0-B674-11B40428107F}"/>
+    <hyperlink ref="G4" tooltip="Manufacturer" display="'" xr:uid="{ECF60CAC-9526-456D-B1EA-10BAAD4226FB}"/>
+    <hyperlink ref="L4" tooltip="Supplier" display="'490-10510-1-ND" xr:uid="{E705977D-4124-4A86-ADCC-9233C52B45F6}"/>
+    <hyperlink ref="F5" tooltip="Component" display="'" xr:uid="{3C792EC4-9967-4943-B132-8DCB3A284A2F}"/>
+    <hyperlink ref="G5" tooltip="Manufacturer" display="'" xr:uid="{7584970C-BD3D-46E1-9F18-BAC5E005FAD6}"/>
+    <hyperlink ref="L5" tooltip="Supplier" display="'490-7229-2-ND" xr:uid="{5B05A9F0-FD29-45F3-BB55-0655E86FF645}"/>
+    <hyperlink ref="F6" tooltip="Component" display="'" xr:uid="{E48464BC-57AF-4720-96F6-6566522BCF04}"/>
+    <hyperlink ref="G6" tooltip="Manufacturer" display="'" xr:uid="{9D7151CF-4F91-4EBF-BBA8-8BF573255DA4}"/>
+    <hyperlink ref="L6" tooltip="Supplier" display="'587-3766-1-ND" xr:uid="{EFBC82BD-DC98-4688-813D-3D29EA4AAB36}"/>
+    <hyperlink ref="F7" tooltip="Component" display="'" xr:uid="{FECF5628-3C51-4FB3-AC88-8DC9B037F5D3}"/>
+    <hyperlink ref="G7" tooltip="Manufacturer" display="'" xr:uid="{62A9F73F-A9E3-4A7A-8317-3ABD0C183867}"/>
+    <hyperlink ref="L7" tooltip="Supplier" display="'311-1047-2-ND" xr:uid="{D70E1B01-2B58-4544-B6DF-15E2D51281CE}"/>
+    <hyperlink ref="F8" tooltip="Component" display="'" xr:uid="{84BD860D-71FA-47AC-95D5-D2E4EA28DDA2}"/>
+    <hyperlink ref="G8" tooltip="Manufacturer" display="'" xr:uid="{F0DE9FED-ADC4-451E-BA53-60A4B28B1AAD}"/>
+    <hyperlink ref="L8" tooltip="Supplier" display="'445-6007-2-ND" xr:uid="{E6B8B8C0-8B66-4D73-AF23-09CFA4440C06}"/>
+    <hyperlink ref="F9" tooltip="Component" display="'" xr:uid="{9FD8BF02-C9DB-4120-8F87-31351F9CE456}"/>
+    <hyperlink ref="G9" tooltip="Manufacturer" display="'" xr:uid="{DAD94241-90BE-4343-814B-B89BAA1BBC5D}"/>
+    <hyperlink ref="L9" tooltip="Supplier" display="'587-3766-1-ND" xr:uid="{DB188016-5EAB-4800-B887-0C8248F69092}"/>
+    <hyperlink ref="F10" tooltip="Component" display="'" xr:uid="{9168315E-4598-448D-9895-1D48C5D6F7BD}"/>
+    <hyperlink ref="G10" tooltip="Manufacturer" display="'" xr:uid="{61466DCF-D7C8-4937-8CC7-FC58A8727154}"/>
+    <hyperlink ref="L10" tooltip="Supplier" display="'445-7438-1-ND, 445-7438-6-ND" xr:uid="{50B6D85A-8B99-49B2-A3D1-D0FFB6F757F4}"/>
+    <hyperlink ref="F11" tooltip="Component" display="'" xr:uid="{1FDDCC77-EC35-4A59-9040-7F95BEF09985}"/>
+    <hyperlink ref="G11" tooltip="Manufacturer" display="'" xr:uid="{458FE05C-103D-4030-99AA-7A46C5822B48}"/>
+    <hyperlink ref="L11" tooltip="Supplier" display="'455-1580-2-ND" xr:uid="{9FA346A2-5E52-49C2-9D74-D09F52D7BB90}"/>
+    <hyperlink ref="F12" tooltip="Component" display="'" xr:uid="{D080A337-08DC-4474-8DA5-8165500B64A2}"/>
+    <hyperlink ref="G12" tooltip="Manufacturer" display="'" xr:uid="{B5B8B789-96D7-4729-B2D8-9B43B3C3263A}"/>
+    <hyperlink ref="L12" tooltip="Supplier" display="'455-1566-2-ND" xr:uid="{CB83A95E-AB5E-4B52-B2EF-00C70FB342E2}"/>
+    <hyperlink ref="F13" tooltip="Component" display="'" xr:uid="{B0B864E2-3767-4C7F-B7F9-0FE7DB5218FC}"/>
+    <hyperlink ref="G13" tooltip="Manufacturer" display="'" xr:uid="{6DDD0B33-4628-4D95-9FC6-57D4772E6A8A}"/>
+    <hyperlink ref="L13" tooltip="Supplier" display="'754-1802-1-ND" xr:uid="{C753D18E-EF44-4FFC-8874-E22B9467F2FA}"/>
+    <hyperlink ref="F14" tooltip="Component" display="'" xr:uid="{6A9363DB-B97E-4459-B8B1-61D98FF80067}"/>
+    <hyperlink ref="G14" tooltip="Manufacturer" display="'" xr:uid="{11F5B3D3-E4D2-48C8-BBFF-C04CBB5468B7}"/>
+    <hyperlink ref="L14" tooltip="Supplier" display="'SM06B-SURS-TF(LF)(SN)-ND" xr:uid="{CE311532-4D09-41D1-A1AD-77BC3D1AFA09}"/>
+    <hyperlink ref="F15" tooltip="Component" display="'" xr:uid="{4FE397CC-4F5E-462B-8998-BF10F870E170}"/>
+    <hyperlink ref="G15" tooltip="Manufacturer" display="'" xr:uid="{F4921511-1E7E-4005-AAFC-D10A4C4DC372}"/>
+    <hyperlink ref="L15" tooltip="Supplier" display="'P15980TR-ND" xr:uid="{F1B6A0BF-ED7A-4026-A4B2-E0D37CD81B80}"/>
+    <hyperlink ref="F16" tooltip="Component" display="'" xr:uid="{C6318181-914F-4948-AC54-A32D67D5078D}"/>
+    <hyperlink ref="G16" tooltip="Manufacturer" display="'" xr:uid="{BCE1EB27-FD96-4D60-93C5-B5DDC90DBC3A}"/>
+    <hyperlink ref="L16" tooltip="Supplier" display="'311-220LRCT-ND" xr:uid="{2F4B0F5D-AD0A-4BDC-B1A3-50D8EBE16FBE}"/>
+    <hyperlink ref="F17" tooltip="Component" display="'" xr:uid="{C5567430-60AB-4A72-83B2-6A3F98CD1C3D}"/>
+    <hyperlink ref="G17" tooltip="Manufacturer" display="'" xr:uid="{E8C5306B-9E6B-4B4F-AD02-54DD30377F94}"/>
+    <hyperlink ref="L17" tooltip="Supplier" display="'311-1.00KLRCT-ND" xr:uid="{67E08871-9FEC-4565-B340-60243EE5FA94}"/>
+    <hyperlink ref="F18" tooltip="Component" display="'" xr:uid="{AE7CB061-B7C3-4065-AB9F-0D6139A0CB9D}"/>
+    <hyperlink ref="G18" tooltip="Manufacturer" display="'" xr:uid="{298CC536-6BAD-49B8-AEB6-AE9ADFD96DED}"/>
+    <hyperlink ref="L18" tooltip="Supplier" display="'311-10.0KLRCT-ND" xr:uid="{AF848C62-7B32-46E0-8342-C52436CF65E6}"/>
+    <hyperlink ref="F19" tooltip="Component" display="'" xr:uid="{3FFB4601-555C-475E-B7DC-0E2E860AD5DE}"/>
+    <hyperlink ref="G19" tooltip="Manufacturer" display="'" xr:uid="{AFEC2D4D-186D-44BB-9848-BA4598116910}"/>
+    <hyperlink ref="L19" tooltip="Supplier" display="'311-120JRTR-ND" xr:uid="{8CD8BC79-F7F4-435F-8AFA-396F4C82F233}"/>
+    <hyperlink ref="F20" tooltip="Component" display="'" xr:uid="{E72C480B-75A0-411E-BA5B-09B6D25589EC}"/>
+    <hyperlink ref="G20" tooltip="Manufacturer" display="'" xr:uid="{300FDA89-E22B-4E57-827D-C0AC1213ACC7}"/>
+    <hyperlink ref="L20" tooltip="Supplier" display="'576-3680-1-ND" xr:uid="{B7AD6552-1D41-43CE-BDAD-7274B67519D1}"/>
+    <hyperlink ref="F21" tooltip="Component" display="'" xr:uid="{2B111D86-23C8-4ADD-B195-914C514200BE}"/>
+    <hyperlink ref="G21" tooltip="Manufacturer" display="'" xr:uid="{61E03B1C-B945-4597-97F4-9029D1011883}"/>
+    <hyperlink ref="L21" tooltip="Supplier" display="'2393651" xr:uid="{3AF9D22C-A3DF-42C4-A6A6-401B2FC23186}"/>
+    <hyperlink ref="F22" tooltip="Component" display="'" xr:uid="{1A5023D7-AE27-4726-9D3F-1E12A648FCCB}"/>
+    <hyperlink ref="G22" tooltip="Manufacturer" display="'" xr:uid="{91075957-ABAD-4EFA-9402-726CB2778E65}"/>
+    <hyperlink ref="L22" tooltip="Supplier" display="'568-8686-2-ND" xr:uid="{FCB7CA1A-2C53-4579-BC3E-64CAB61565BE}"/>
+    <hyperlink ref="F23" tooltip="Component" display="'" xr:uid="{1E438BA4-5C06-4FFC-904D-FF0923AF6573}"/>
+    <hyperlink ref="G23" tooltip="Manufacturer" display="'" xr:uid="{03D6C3CA-02F5-403A-BDC3-45DAFBAAADCE}"/>
+    <hyperlink ref="L23" tooltip="Supplier" display="'NUF2042XV6T1GOSDKR-ND" xr:uid="{3A11F73D-6203-429D-8C00-0908A7F51117}"/>
+    <hyperlink ref="F24" tooltip="Component" display="'" xr:uid="{1B6E1A15-6D19-4915-9DB0-CC62C10E2CDD}"/>
+    <hyperlink ref="G24" tooltip="Manufacturer" display="'" xr:uid="{F88C5458-3B55-4220-AE30-075B00595EB7}"/>
+    <hyperlink ref="L24" tooltip="Supplier" display="'" xr:uid="{800EB1FA-A144-4FED-ACAB-9ED4BE3DBA0A}"/>
+    <hyperlink ref="F25" tooltip="Component" display="'" xr:uid="{3E8B4FD7-CCF6-43AE-BB6F-A4BBB42D41DC}"/>
+    <hyperlink ref="G25" tooltip="Manufacturer" display="'" xr:uid="{F7C9A90C-3ACD-4089-A187-273E0D5F5FFB}"/>
+    <hyperlink ref="L25" tooltip="Supplier" display="'1479-1002-2-ND" xr:uid="{108F8239-EC15-475D-94FA-24785E02D44F}"/>
+    <hyperlink ref="F26" tooltip="Component" display="'" xr:uid="{869DD71A-0DEE-41E8-AD43-390B26A2907C}"/>
+    <hyperlink ref="G26" tooltip="Manufacturer" display="'" xr:uid="{D3CB8E9A-EF3B-496B-BA22-79B8B923579A}"/>
+    <hyperlink ref="L26" tooltip="Supplier" display="'887-1846-2-ND" xr:uid="{C9B5C885-42B3-404A-A7B5-A06152D5E020}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>